<commit_message>
updated to word by word parsing
</commit_message>
<xml_diff>
--- a/data/metadata_corrected.xlsx
+++ b/data/metadata_corrected.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikekestemont/GitRepos/mdu/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06ACD857-E649-2546-9B2F-DFF204AE2FB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91A1927-5D37-A14F-9E4C-160CE62B3659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1754" uniqueCount="603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1756" uniqueCount="603">
   <si>
     <t>id</t>
   </si>
@@ -2228,8 +2228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I284"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="H110" sqref="H110"/>
+    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
+      <selection activeCell="I192" sqref="I192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6317,7 +6317,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
         <v>331</v>
       </c>
@@ -6343,7 +6343,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>360</v>
       </c>
@@ -6369,7 +6369,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
         <v>50</v>
       </c>
@@ -6389,7 +6389,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>202</v>
       </c>
@@ -6412,7 +6412,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
         <v>18</v>
       </c>
@@ -6435,7 +6435,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
         <v>181</v>
       </c>
@@ -6458,7 +6458,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
         <v>248</v>
       </c>
@@ -6481,7 +6481,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
         <v>336</v>
       </c>
@@ -6504,7 +6504,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
         <v>372</v>
       </c>
@@ -6527,7 +6527,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
         <v>311</v>
       </c>
@@ -6550,7 +6550,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
         <v>177</v>
       </c>
@@ -6573,7 +6573,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
         <v>244</v>
       </c>
@@ -6596,7 +6596,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
         <v>329</v>
       </c>
@@ -6619,7 +6619,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
         <v>391</v>
       </c>
@@ -6642,7 +6642,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
         <v>200</v>
       </c>
@@ -6664,8 +6664,11 @@
       <c r="H191" t="s">
         <v>596</v>
       </c>
-    </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I191" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
         <v>293</v>
       </c>
@@ -6686,6 +6689,9 @@
       </c>
       <c r="H192" t="s">
         <v>596</v>
+      </c>
+      <c r="I192" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
set correct main version of Wrake
</commit_message>
<xml_diff>
--- a/data/metadata_corrected.xlsx
+++ b/data/metadata_corrected.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikekestemont/GitRepos/mdu/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F206F1-8D3A-8A4E-B4CF-715FDFF502E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7758AA-B2CD-0F41-83E2-E030789F4C1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2231,8 +2231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="F87" sqref="F87"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6034,6 +6034,9 @@
       <c r="H164" t="s">
         <v>553</v>
       </c>
+      <c r="I164" t="s">
+        <v>570</v>
+      </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
@@ -6082,9 +6085,6 @@
       </c>
       <c r="H166" t="s">
         <v>553</v>
-      </c>
-      <c r="I166" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>